<commit_message>
2024-07-10: coding in CNN_Model_Functions.py
</commit_message>
<xml_diff>
--- a/Calculator for CNN.xlsx
+++ b/Calculator for CNN.xlsx
@@ -7,7 +7,7 @@
     <workbookView windowWidth="28800" windowHeight="11460"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LeNet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,66 +27,392 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
-    <t>层数</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>层数</t>
+    </r>
   </si>
   <si>
-    <t>输入</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>输入</t>
+    </r>
   </si>
   <si>
-    <t>滤波器</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>滤波器</t>
+    </r>
   </si>
   <si>
-    <t>输出</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>输出</t>
+    </r>
   </si>
   <si>
-    <t>通道数（C）</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>通道数（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
   </si>
   <si>
-    <t>高度(H)</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>高度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(H)</t>
+    </r>
   </si>
   <si>
-    <t>宽度（W)</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>宽度（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>W)</t>
+    </r>
   </si>
   <si>
-    <t>滤波器个数（FN）</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>滤波器个数（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>FN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
   </si>
   <si>
-    <t>大小（Kernel size）</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>大小（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Kernel size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
   </si>
   <si>
-    <t>步幅（Stride）</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>步幅（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Stride</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
   </si>
   <si>
-    <t>填充（Padding）</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>填充（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Padding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
   </si>
   <si>
-    <t>输入层</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>输入层</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>卷积层</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>池化层</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
   </si>
   <si>
     <t>/</t>
   </si>
   <si>
-    <t>卷积层1</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>卷积层</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
   </si>
   <si>
-    <t>池化层1</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>池化层</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
   </si>
   <si>
-    <t>卷积层2</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>卷积层</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
   </si>
   <si>
-    <t>池化层2</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>全连接层</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
   </si>
   <si>
-    <t>卷积层3</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>全连接层</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
   </si>
   <si>
-    <t>全连接层1</t>
-  </si>
-  <si>
-    <t>全连接层2</t>
+    <t>输出层</t>
   </si>
 </sst>
 </file>
@@ -99,7 +425,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,9 +436,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Times Regular"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体-简"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -258,8 +589,14 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +612,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -649,55 +992,52 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -712,70 +1052,73 @@
     <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -792,35 +1135,35 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1347,20 +1690,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="22.6923076923077" customWidth="1"/>
-    <col min="2" max="9" width="16.6923076923077" customWidth="1"/>
-    <col min="10" max="12" width="18.6923076923077" customWidth="1"/>
+    <col min="2" max="13" width="14.6923076923077" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:12">
+    <row r="1" ht="25" customHeight="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1369,20 +1711,21 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="11" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
     </row>
-    <row r="2" ht="37" customHeight="1" spans="1:12">
+    <row r="2" ht="37" customHeight="1" spans="1:13">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -1393,258 +1736,416 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="20" customHeight="1" spans="1:12">
+    <row r="3" ht="20" customHeight="1" spans="1:13">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="9" t="s">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>56</v>
+      </c>
+      <c r="D3" s="4">
+        <v>56</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" ht="20" customHeight="1" spans="1:13">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>12</v>
+      <c r="B4" s="2">
+        <f>B3</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <f>C3</f>
+        <v>56</v>
+      </c>
+      <c r="D4" s="2">
+        <f>D3</f>
+        <v>56</v>
+      </c>
+      <c r="E4" s="10">
+        <v>6</v>
+      </c>
+      <c r="F4" s="10">
+        <f>B3</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="10">
+        <v>6</v>
+      </c>
+      <c r="H4" s="10">
+        <v>6</v>
+      </c>
+      <c r="I4" s="10">
+        <v>2</v>
+      </c>
+      <c r="J4" s="10">
+        <v>2</v>
+      </c>
+      <c r="K4" s="12">
+        <f t="shared" ref="K4:K9" si="0">E4</f>
+        <v>6</v>
+      </c>
+      <c r="L4" s="12">
+        <f t="shared" ref="L4:L8" si="1">(C4+2*$J4-G4)/$I4+1</f>
+        <v>28</v>
+      </c>
+      <c r="M4" s="12">
+        <f t="shared" ref="M4:M8" si="2">(D4+2*$J4-H4)/$I4+1</f>
+        <v>28</v>
       </c>
     </row>
-    <row r="4" ht="20" customHeight="1" spans="1:12">
-      <c r="A4" s="4" t="s">
+    <row r="5" ht="20" customHeight="1" spans="1:13">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9">
-        <f>B3</f>
+      <c r="B5" s="2">
+        <f t="shared" ref="B5:B10" si="3">K4</f>
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" ref="C5:C10" si="4">L4</f>
+        <v>28</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" ref="D5:D10" si="5">M4</f>
+        <v>28</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="10">
+        <v>2</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" ref="H4:H8" si="6">G5</f>
+        <v>2</v>
+      </c>
+      <c r="I5" s="10">
+        <v>2</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="12">
+        <f>B5</f>
+        <v>6</v>
+      </c>
+      <c r="L5" s="12">
+        <f>C5/$I5</f>
+        <v>14</v>
+      </c>
+      <c r="M5" s="12">
+        <f>D5/$I5</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1" spans="1:13">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="E6" s="10">
+        <v>16</v>
+      </c>
+      <c r="F6" s="10">
+        <f>B5</f>
+        <v>6</v>
+      </c>
+      <c r="G6" s="10">
+        <v>5</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="I6" s="10">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10">
         <v>0</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="13">
-        <f>E4</f>
+      <c r="K6" s="12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="L6" s="12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M6" s="12">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1" spans="1:13">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="10">
+        <v>2</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="I7" s="10">
+        <v>1</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="12">
+        <f>B7</f>
+        <v>16</v>
+      </c>
+      <c r="L7" s="12">
+        <f>C7/$I7</f>
+        <v>10</v>
+      </c>
+      <c r="M7" s="12">
+        <f>D7/$I7</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1" spans="1:13">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="10">
+        <v>120</v>
+      </c>
+      <c r="F8" s="10">
+        <f>B7</f>
+        <v>16</v>
+      </c>
+      <c r="G8" s="10">
+        <v>10</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I8" s="10">
+        <v>1</v>
+      </c>
+      <c r="J8" s="10">
         <v>0</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="K8" s="12">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="L8" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M8" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" ht="20" customHeight="1" spans="1:12">
-      <c r="A5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9">
-        <f t="shared" ref="F5:F11" si="0">B4</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="13">
-        <f>E5</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
+    <row r="9" ht="20" customHeight="1" spans="1:13">
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="12">
+        <v>84</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" ht="20" customHeight="1" spans="1:12">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="13">
-        <f>E6</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
+    <row r="10" ht="20" customHeight="1" spans="1:13">
+      <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>/</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>/</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="12">
+        <v>10</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="7" ht="20" customHeight="1" spans="1:12">
-      <c r="A7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="13">
-        <f>E7</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-    </row>
-    <row r="8" ht="20" customHeight="1" spans="1:12">
-      <c r="A8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="13">
-        <f>E8</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-    </row>
-    <row r="9" ht="20" customHeight="1" spans="1:12">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="13">
-        <f>E9</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-    </row>
-    <row r="10" ht="20" customHeight="1" spans="1:12">
-      <c r="A10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-    </row>
-    <row r="11" ht="20" customHeight="1" spans="1:12">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-    </row>
-    <row r="12" ht="20" customHeight="1" spans="1:12">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-    </row>
-    <row r="13" ht="20" customHeight="1" spans="1:12">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
+    <row r="11" ht="20" customHeight="1" spans="1:13">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4">
+        <f>K10</f>
+        <v>10</v>
+      </c>
+      <c r="L11" s="4" t="str">
+        <f>L10</f>
+        <v>/</v>
+      </c>
+      <c r="M11" s="4" t="str">
+        <f>M10</f>
+        <v>/</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="K1:M1"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>